<commit_message>
Split Smoke Test Suite into Multiple function suites.
</commit_message>
<xml_diff>
--- a/PublishScriptData.xlsx
+++ b/PublishScriptData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njones\Katalon Studio\Convergence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E157C601-9524-45EE-8F42-C61E34911D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AD17F4-69A1-4AE2-99C3-DACA953B4C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{075BFB0F-00A9-4E7B-8038-832DAC2B2BC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{075BFB0F-00A9-4E7B-8038-832DAC2B2BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="TDES" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Template Name</t>
   </si>
@@ -88,9 +88,6 @@
     <t>PDFCompressor</t>
   </si>
   <si>
-    <t>PDFTools</t>
-  </si>
-  <si>
     <t>PDFUtil</t>
   </si>
   <si>
@@ -145,25 +142,16 @@
     <t>Test - TempFile - PdfUtils</t>
   </si>
   <si>
-    <t>Test - TempFile - SMBV2FileTransferUtils</t>
-  </si>
-  <si>
     <t>Test - TempFile - WordUtil - WordConvertFieldsToText</t>
   </si>
   <si>
     <t>Test - TempFile - WordUtil - WordDocumentHeader</t>
   </si>
   <si>
-    <t>TestSuite - TempFile</t>
-  </si>
-  <si>
     <t>Tiff2Pdf</t>
   </si>
   <si>
     <t>XMLTransform</t>
-  </si>
-  <si>
-    <t>codecutil</t>
   </si>
 </sst>
 </file>
@@ -550,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E5AE8C-C25F-4AC7-92DB-754258779606}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,33 +571,28 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" tooltip="Click to edit template" display="http://localhost:8087/tdes/console/getTemplateList" xr:uid="{A6F5E459-75FF-46AF-B939-AACEAD6BA475}"/>
-    <hyperlink ref="A8" r:id="rId2" tooltip="Click to edit template" display="http://localhost:8087/tdes/console/getTemplateList" xr:uid="{ADE0DBF1-6828-47B6-B6D7-00A489EFF7F8}"/>
+    <hyperlink ref="A6" r:id="rId1" tooltip="Click to edit template" display="http://localhost:8087/tdes/console/getTemplateList" xr:uid="{A6F5E459-75FF-46AF-B939-AACEAD6BA475}"/>
+    <hyperlink ref="A7" r:id="rId2" tooltip="Click to edit template" display="http://localhost:8087/tdes/console/getTemplateList" xr:uid="{ADE0DBF1-6828-47B6-B6D7-00A489EFF7F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -617,10 +600,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C590552D-DD0B-4B45-8556-28E056107D05}">
-  <dimension ref="A1:A47"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,12 +761,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -800,58 +783,43 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A42" s="1"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates for 21 release
</commit_message>
<xml_diff>
--- a/PublishScriptData.xlsx
+++ b/PublishScriptData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njones\Katalon Studio\Convergence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AD17F4-69A1-4AE2-99C3-DACA953B4C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE291BDB-0009-4019-BE36-B194F44C310D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{075BFB0F-00A9-4E7B-8038-832DAC2B2BC7}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{075BFB0F-00A9-4E7B-8038-832DAC2B2BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="TDES" sheetId="1" r:id="rId1"/>
     <sheet name="CV" sheetId="3" r:id="rId2"/>
+    <sheet name="bak" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>Template Name</t>
   </si>
@@ -600,10 +601,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C590552D-DD0B-4B45-8556-28E056107D05}">
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,6 +634,209 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3A2CD8-C36F-4E87-8DCC-AA9609FD4505}">
+  <dimension ref="A1:A44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Several updates made to test cases and suites against TDES 21.
</commit_message>
<xml_diff>
--- a/PublishScriptData.xlsx
+++ b/PublishScriptData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njones\Katalon Studio\Convergence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE291BDB-0009-4019-BE36-B194F44C310D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFE1759-9B2B-4E4D-BFC0-7AC159DB8B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{075BFB0F-00A9-4E7B-8038-832DAC2B2BC7}"/>
+    <workbookView xWindow="19090" yWindow="-180" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{075BFB0F-00A9-4E7B-8038-832DAC2B2BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="TDES" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>Template Name</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>XMLTransform</t>
+  </si>
+  <si>
+    <t>docgen-pdf-template-fill</t>
   </si>
 </sst>
 </file>
@@ -545,47 +548,47 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -603,202 +606,205 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C590552D-DD0B-4B45-8556-28E056107D05}">
   <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="50.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -810,219 +816,219 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="50.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
     </row>
   </sheetData>

</xml_diff>